<commit_message>
Update anotated result, location and time analysis
</commit_message>
<xml_diff>
--- a/erupsi/v02-new/sample_erupsi_anotasi_v02_new.xlsx
+++ b/erupsi/v02-new/sample_erupsi_anotasi_v02_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dharmapu\Documents\personal\ui\KA-AMSD_src\paper-submission\anotated_data\erupsi\v02-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FFB053-2E80-45F7-89DF-E5FB00968DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4369550E-5947-4D63-B622-1B364DAB975F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8983" uniqueCount="1717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8983" uniqueCount="1715">
   <si>
     <t>id</t>
   </si>
@@ -4876,13 +4876,7 @@
     <t>Kalipuro</t>
   </si>
   <si>
-    <t>Kabupaten NULL</t>
-  </si>
-  <si>
     <t>Bandara Blimbingsari</t>
-  </si>
-  <si>
-    <t>NUll</t>
   </si>
   <si>
     <t xml:space="preserve">Bandara Ngurai Rai </t>
@@ -6182,8 +6176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1366" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1375" sqref="D1375"/>
+    <sheetView tabSelected="1" topLeftCell="A1289" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G1305" sqref="G1305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6943,7 +6937,7 @@
         <v>1167</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>1276</v>
@@ -6955,14 +6949,14 @@
         <v>1182</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -6976,7 +6970,7 @@
         <v>1167</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>1276</v>
@@ -6988,14 +6982,14 @@
         <v>1182</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7009,7 +7003,7 @@
         <v>1167</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>1276</v>
@@ -7021,14 +7015,14 @@
         <v>1182</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7042,7 +7036,7 @@
         <v>1167</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>1276</v>
@@ -7054,14 +7048,14 @@
         <v>1182</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7075,7 +7069,7 @@
         <v>1167</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>1276</v>
@@ -7087,14 +7081,14 @@
         <v>1182</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7108,7 +7102,7 @@
         <v>1167</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>1276</v>
@@ -7117,17 +7111,17 @@
         <v>1364</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7141,7 +7135,7 @@
         <v>1167</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>1276</v>
@@ -7150,17 +7144,17 @@
         <v>1364</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7174,7 +7168,7 @@
         <v>1167</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>1276</v>
@@ -7193,7 +7187,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7207,7 +7201,7 @@
         <v>1167</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>1276</v>
@@ -7219,14 +7213,14 @@
         <v>1515</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7240,7 +7234,7 @@
         <v>1167</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>1276</v>
@@ -7252,14 +7246,14 @@
         <v>1515</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7273,7 +7267,7 @@
         <v>1167</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>1276</v>
@@ -7285,14 +7279,14 @@
         <v>1515</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7306,7 +7300,7 @@
         <v>1167</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>1276</v>
@@ -7325,7 +7319,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7339,7 +7333,7 @@
         <v>1167</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>1276</v>
@@ -7351,14 +7345,14 @@
         <v>1515</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7372,7 +7366,7 @@
         <v>1167</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>1276</v>
@@ -7391,7 +7385,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7405,7 +7399,7 @@
         <v>1167</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>1276</v>
@@ -7417,14 +7411,14 @@
         <v>1182</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7438,7 +7432,7 @@
         <v>1167</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>1276</v>
@@ -7450,14 +7444,14 @@
         <v>1182</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7471,7 +7465,7 @@
         <v>1167</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>1276</v>
@@ -7480,17 +7474,17 @@
         <v>1364</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -7504,7 +7498,7 @@
         <v>1167</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>1276</v>
@@ -7516,14 +7510,14 @@
         <v>1182</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -8057,7 +8051,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
       <c r="M70" s="5" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -8266,7 +8260,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
       <c r="M77" s="5" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -8292,14 +8286,14 @@
         <v>1347</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
       <c r="M78" s="5" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -8923,10 +8917,10 @@
         <v>1296</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="I102" s="5"/>
       <c r="J102" s="5"/>
@@ -9001,7 +8995,7 @@
         <v>1167</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>1196</v>
@@ -9013,7 +9007,7 @@
         <v>1213</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
@@ -9116,7 +9110,7 @@
       <c r="K109" s="5"/>
       <c r="L109" s="5"/>
       <c r="M109" s="5" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -9149,7 +9143,7 @@
       <c r="K110" s="5"/>
       <c r="L110" s="5"/>
       <c r="M110" s="5" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -9182,7 +9176,7 @@
       <c r="K111" s="5"/>
       <c r="L111" s="5"/>
       <c r="M111" s="5" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -9215,7 +9209,7 @@
       <c r="K112" s="5"/>
       <c r="L112" s="5"/>
       <c r="M112" s="5" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -9248,7 +9242,7 @@
       <c r="K113" s="5"/>
       <c r="L113" s="5"/>
       <c r="M113" s="5" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -9281,7 +9275,7 @@
       <c r="K114" s="5"/>
       <c r="L114" s="5"/>
       <c r="M114" s="5" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -12257,7 +12251,7 @@
         <v>1167</v>
       </c>
       <c r="D245" s="7" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="E245" s="5" t="s">
         <v>1185</v>
@@ -12276,7 +12270,7 @@
       <c r="K245" s="5"/>
       <c r="L245" s="5"/>
       <c r="M245" s="5" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.25">
@@ -14774,20 +14768,20 @@
         <v>1276</v>
       </c>
       <c r="F340" s="5" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="G340" s="5" t="s">
         <v>1567</v>
       </c>
       <c r="H340" s="5" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="I340" s="5"/>
       <c r="J340" s="5"/>
       <c r="K340" s="5"/>
       <c r="L340" s="5"/>
       <c r="M340" s="5" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.25">
@@ -15954,7 +15948,7 @@
       <c r="K391" s="5"/>
       <c r="L391" s="5"/>
       <c r="M391" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.25">
@@ -16521,7 +16515,7 @@
       <c r="K414" s="5"/>
       <c r="L414" s="5"/>
       <c r="M414" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="415" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16554,7 +16548,7 @@
       <c r="K415" s="5"/>
       <c r="L415" s="5"/>
       <c r="M415" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="416" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16587,7 +16581,7 @@
       <c r="K416" s="5"/>
       <c r="L416" s="5"/>
       <c r="M416" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="417" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16613,14 +16607,14 @@
         <v>1182</v>
       </c>
       <c r="H417" s="5" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="I417" s="5"/>
       <c r="J417" s="5"/>
       <c r="K417" s="5"/>
       <c r="L417" s="5"/>
       <c r="M417" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="418" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16646,14 +16640,14 @@
         <v>1182</v>
       </c>
       <c r="H418" s="5" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="I418" s="5"/>
       <c r="J418" s="5"/>
       <c r="K418" s="5"/>
       <c r="L418" s="5"/>
       <c r="M418" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="419" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16679,14 +16673,14 @@
         <v>1182</v>
       </c>
       <c r="H419" s="5" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="I419" s="5"/>
       <c r="J419" s="5"/>
       <c r="K419" s="5"/>
       <c r="L419" s="5"/>
       <c r="M419" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="420" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16712,14 +16706,14 @@
         <v>1182</v>
       </c>
       <c r="H420" s="5" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="I420" s="5"/>
       <c r="J420" s="5"/>
       <c r="K420" s="5"/>
       <c r="L420" s="5"/>
       <c r="M420" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="421" spans="1:13" x14ac:dyDescent="0.25">
@@ -16775,7 +16769,7 @@
         <v>1167</v>
       </c>
       <c r="D423" s="7" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="E423" s="5" t="s">
         <v>1254</v>
@@ -16794,7 +16788,7 @@
       <c r="K423" s="5"/>
       <c r="L423" s="5"/>
       <c r="M423" s="5" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="424" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -16827,7 +16821,7 @@
       <c r="K424" s="5"/>
       <c r="L424" s="5"/>
       <c r="M424" s="5" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.25">
@@ -16935,7 +16929,7 @@
       <c r="K428" s="5"/>
       <c r="L428" s="5"/>
       <c r="M428" s="5" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="429" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -16955,7 +16949,7 @@
         <v>1181</v>
       </c>
       <c r="F429" s="5" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="G429" s="5" t="s">
         <v>1436</v>
@@ -16968,7 +16962,7 @@
       <c r="K429" s="5"/>
       <c r="L429" s="5"/>
       <c r="M429" s="5" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="430" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -17001,7 +16995,7 @@
       <c r="K430" s="5"/>
       <c r="L430" s="5"/>
       <c r="M430" s="5" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="431" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -17034,7 +17028,7 @@
       <c r="K431" s="5"/>
       <c r="L431" s="5"/>
       <c r="M431" s="5" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="432" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -17067,7 +17061,7 @@
       <c r="K432" s="5"/>
       <c r="L432" s="5"/>
       <c r="M432" s="5" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.25">
@@ -17193,7 +17187,7 @@
         <v>1167</v>
       </c>
       <c r="D437" s="7" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="E437" s="5" t="s">
         <v>1196</v>
@@ -18037,7 +18031,7 @@
       <c r="K472" s="5"/>
       <c r="L472" s="5"/>
       <c r="M472" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="473" spans="1:13" x14ac:dyDescent="0.25">
@@ -18070,7 +18064,7 @@
       <c r="K473" s="5"/>
       <c r="L473" s="5"/>
       <c r="M473" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="474" spans="1:13" x14ac:dyDescent="0.25">
@@ -18103,7 +18097,7 @@
       <c r="K474" s="5"/>
       <c r="L474" s="5"/>
       <c r="M474" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="475" spans="1:13" x14ac:dyDescent="0.25">
@@ -18129,14 +18123,14 @@
         <v>1343</v>
       </c>
       <c r="H475" s="5" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="I475" s="5"/>
       <c r="J475" s="5"/>
       <c r="K475" s="5"/>
       <c r="L475" s="5"/>
       <c r="M475" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="476" spans="1:13" x14ac:dyDescent="0.25">
@@ -18162,14 +18156,14 @@
         <v>1343</v>
       </c>
       <c r="H476" s="5" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="I476" s="5"/>
       <c r="J476" s="5"/>
       <c r="K476" s="5"/>
       <c r="L476" s="5"/>
       <c r="M476" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="477" spans="1:13" x14ac:dyDescent="0.25">
@@ -18202,7 +18196,7 @@
       <c r="K477" s="5"/>
       <c r="L477" s="5"/>
       <c r="M477" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="478" spans="1:13" x14ac:dyDescent="0.25">
@@ -18228,14 +18222,14 @@
         <v>1211</v>
       </c>
       <c r="H478" s="5" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="I478" s="5"/>
       <c r="J478" s="5"/>
       <c r="K478" s="5"/>
       <c r="L478" s="5"/>
       <c r="M478" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="479" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -18258,7 +18252,7 @@
         <v>1198</v>
       </c>
       <c r="G479" s="5" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
       <c r="H479" s="5"/>
       <c r="I479" s="5"/>
@@ -18266,7 +18260,7 @@
       <c r="K479" s="5"/>
       <c r="L479" s="5"/>
       <c r="M479" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="480" spans="1:13" x14ac:dyDescent="0.25">
@@ -18292,14 +18286,14 @@
         <v>1213</v>
       </c>
       <c r="H480" s="5" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="I480" s="5"/>
       <c r="J480" s="5"/>
       <c r="K480" s="5"/>
       <c r="L480" s="5"/>
       <c r="M480" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="481" spans="1:13" x14ac:dyDescent="0.25">
@@ -18325,14 +18319,14 @@
         <v>1213</v>
       </c>
       <c r="H481" s="5" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="I481" s="5"/>
       <c r="J481" s="5"/>
       <c r="K481" s="5"/>
       <c r="L481" s="5"/>
       <c r="M481" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="482" spans="1:13" x14ac:dyDescent="0.25">
@@ -18365,7 +18359,7 @@
       <c r="K482" s="5"/>
       <c r="L482" s="5"/>
       <c r="M482" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="483" spans="1:13" x14ac:dyDescent="0.25">
@@ -18391,14 +18385,14 @@
         <v>1349</v>
       </c>
       <c r="H483" s="5" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="I483" s="5"/>
       <c r="J483" s="5"/>
       <c r="K483" s="5"/>
       <c r="L483" s="5"/>
       <c r="M483" s="5" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="484" spans="1:13" x14ac:dyDescent="0.25">
@@ -18857,7 +18851,7 @@
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
       <c r="M502" s="5" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="503" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -18890,7 +18884,7 @@
       <c r="K503" s="5"/>
       <c r="L503" s="5"/>
       <c r="M503" s="5" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="504" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -18923,7 +18917,7 @@
       <c r="K504" s="5"/>
       <c r="L504" s="5"/>
       <c r="M504" s="5" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="505" spans="1:13" x14ac:dyDescent="0.25">
@@ -19454,7 +19448,7 @@
         <v>1228</v>
       </c>
       <c r="F528" s="5" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="G528" s="5" t="s">
         <v>1182</v>
@@ -20904,7 +20898,7 @@
       <c r="K581" s="5"/>
       <c r="L581" s="5"/>
       <c r="M581" s="5" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="582" spans="1:13" x14ac:dyDescent="0.25">
@@ -22262,16 +22256,16 @@
         <v>1167</v>
       </c>
       <c r="D638" s="7" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="E638" s="5" t="s">
         <v>1283</v>
       </c>
       <c r="F638" s="5" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="G638" s="5" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="H638" s="5" t="s">
         <v>1182</v>
@@ -22281,7 +22275,7 @@
       <c r="K638" s="5"/>
       <c r="L638" s="5"/>
       <c r="M638" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="639" spans="1:13" x14ac:dyDescent="0.25">
@@ -22442,7 +22436,7 @@
         <v>1167</v>
       </c>
       <c r="D646" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E646" s="5" t="s">
         <v>1283</v>
@@ -22454,14 +22448,14 @@
         <v>1285</v>
       </c>
       <c r="H646" s="5" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="I646" s="5"/>
       <c r="J646" s="5"/>
       <c r="K646" s="5"/>
       <c r="L646" s="5"/>
       <c r="M646" s="5" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="647" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22475,7 +22469,7 @@
         <v>1167</v>
       </c>
       <c r="D647" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E647" s="5" t="s">
         <v>1283</v>
@@ -22494,7 +22488,7 @@
       <c r="K647" s="5"/>
       <c r="L647" s="5"/>
       <c r="M647" s="5" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="648" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22508,7 +22502,7 @@
         <v>1167</v>
       </c>
       <c r="D648" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E648" s="5" t="s">
         <v>1283</v>
@@ -22527,7 +22521,7 @@
       <c r="K648" s="5"/>
       <c r="L648" s="5"/>
       <c r="M648" s="5" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="649" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22541,7 +22535,7 @@
         <v>1167</v>
       </c>
       <c r="D649" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E649" s="5" t="s">
         <v>1283</v>
@@ -22560,7 +22554,7 @@
       <c r="K649" s="5"/>
       <c r="L649" s="5"/>
       <c r="M649" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="650" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22574,7 +22568,7 @@
         <v>1167</v>
       </c>
       <c r="D650" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E650" s="5" t="s">
         <v>1283</v>
@@ -22593,7 +22587,7 @@
       <c r="K650" s="5"/>
       <c r="L650" s="5"/>
       <c r="M650" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="651" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22607,7 +22601,7 @@
         <v>1167</v>
       </c>
       <c r="D651" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E651" s="5" t="s">
         <v>1283</v>
@@ -22619,14 +22613,14 @@
         <v>1384</v>
       </c>
       <c r="H651" s="5" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="I651" s="5"/>
       <c r="J651" s="5"/>
       <c r="K651" s="5"/>
       <c r="L651" s="5"/>
       <c r="M651" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="652" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22640,7 +22634,7 @@
         <v>1167</v>
       </c>
       <c r="D652" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E652" s="5" t="s">
         <v>1283</v>
@@ -22652,14 +22646,14 @@
         <v>1385</v>
       </c>
       <c r="H652" s="5" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="I652" s="5"/>
       <c r="J652" s="5"/>
       <c r="K652" s="5"/>
       <c r="L652" s="5"/>
       <c r="M652" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="653" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22673,7 +22667,7 @@
         <v>1167</v>
       </c>
       <c r="D653" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E653" s="5" t="s">
         <v>1283</v>
@@ -22685,14 +22679,14 @@
         <v>1278</v>
       </c>
       <c r="H653" s="5" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="I653" s="5"/>
       <c r="J653" s="5"/>
       <c r="K653" s="5"/>
       <c r="L653" s="5"/>
       <c r="M653" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="654" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22706,7 +22700,7 @@
         <v>1167</v>
       </c>
       <c r="D654" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E654" s="5" t="s">
         <v>1283</v>
@@ -22718,14 +22712,14 @@
         <v>1278</v>
       </c>
       <c r="H654" s="5" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="I654" s="5"/>
       <c r="J654" s="5"/>
       <c r="K654" s="5"/>
       <c r="L654" s="5"/>
       <c r="M654" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="655" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -22739,7 +22733,7 @@
         <v>1167</v>
       </c>
       <c r="D655" s="7" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E655" s="5" t="s">
         <v>1276</v>
@@ -22758,7 +22752,7 @@
       <c r="K655" s="5"/>
       <c r="L655" s="5"/>
       <c r="M655" s="5" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="656" spans="1:13" x14ac:dyDescent="0.25">
@@ -23828,7 +23822,7 @@
         <v>1167</v>
       </c>
       <c r="D704" s="7" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="E704" s="5" t="s">
         <v>1254</v>
@@ -23847,7 +23841,7 @@
       <c r="K704" s="5"/>
       <c r="L704" s="5"/>
       <c r="M704" s="5" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="705" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -23861,13 +23855,13 @@
         <v>1167</v>
       </c>
       <c r="D705" s="7" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="E705" s="5" t="s">
         <v>1254</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="G705" s="5" t="s">
         <v>1182</v>
@@ -23880,7 +23874,7 @@
       <c r="K705" s="5"/>
       <c r="L705" s="5"/>
       <c r="M705" s="5" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="706" spans="1:13" x14ac:dyDescent="0.25">
@@ -24017,7 +24011,7 @@
         <v>1254</v>
       </c>
       <c r="F711" s="5" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="G711" s="5" t="s">
         <v>1182</v>
@@ -24104,7 +24098,7 @@
         <v>1254</v>
       </c>
       <c r="F714" s="5" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="G714" s="5" t="s">
         <v>1182</v>
@@ -24191,7 +24185,7 @@
         <v>1254</v>
       </c>
       <c r="F717" s="5" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="G717" s="5" t="s">
         <v>1182</v>
@@ -24919,7 +24913,7 @@
         <v>1560</v>
       </c>
       <c r="H745" s="5" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="I745" s="5"/>
       <c r="J745" s="5"/>
@@ -24952,7 +24946,7 @@
         <v>1343</v>
       </c>
       <c r="H746" s="5" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="I746" s="5"/>
       <c r="J746" s="5"/>
@@ -25018,7 +25012,7 @@
         <v>1347</v>
       </c>
       <c r="H748" s="5" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="I748" s="5"/>
       <c r="J748" s="5"/>
@@ -25051,7 +25045,7 @@
         <v>1560</v>
       </c>
       <c r="H749" s="5" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="I749" s="5"/>
       <c r="J749" s="5"/>
@@ -25135,7 +25129,7 @@
         <v>10000</v>
       </c>
       <c r="M752" s="5" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="753" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -30037,7 +30031,7 @@
       <c r="K952" s="5"/>
       <c r="L952" s="5"/>
       <c r="M952" s="5" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="953" spans="1:13" x14ac:dyDescent="0.25">
@@ -30093,7 +30087,7 @@
         <v>1167</v>
       </c>
       <c r="D955" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E955" s="5" t="s">
         <v>1182</v>
@@ -30126,7 +30120,7 @@
         <v>1167</v>
       </c>
       <c r="D956" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E956" s="5" t="s">
         <v>1276</v>
@@ -30159,7 +30153,7 @@
         <v>1167</v>
       </c>
       <c r="D957" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E957" s="5" t="s">
         <v>1276</v>
@@ -30192,7 +30186,7 @@
         <v>1167</v>
       </c>
       <c r="D958" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E958" s="5" t="s">
         <v>1276</v>
@@ -30225,7 +30219,7 @@
         <v>1167</v>
       </c>
       <c r="D959" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E959" s="5" t="s">
         <v>1276</v>
@@ -30258,7 +30252,7 @@
         <v>1167</v>
       </c>
       <c r="D960" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E960" s="5" t="s">
         <v>1276</v>
@@ -30291,7 +30285,7 @@
         <v>1167</v>
       </c>
       <c r="D961" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E961" s="5" t="s">
         <v>1276</v>
@@ -30324,7 +30318,7 @@
         <v>1167</v>
       </c>
       <c r="D962" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E962" s="5" t="s">
         <v>1276</v>
@@ -30357,7 +30351,7 @@
         <v>1167</v>
       </c>
       <c r="D963" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E963" s="5" t="s">
         <v>1276</v>
@@ -30390,7 +30384,7 @@
         <v>1167</v>
       </c>
       <c r="D964" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E964" s="5" t="s">
         <v>1276</v>
@@ -30423,7 +30417,7 @@
         <v>1167</v>
       </c>
       <c r="D965" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E965" s="5" t="s">
         <v>1276</v>
@@ -30456,7 +30450,7 @@
         <v>1167</v>
       </c>
       <c r="D966" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E966" s="5" t="s">
         <v>1276</v>
@@ -30489,7 +30483,7 @@
         <v>1167</v>
       </c>
       <c r="D967" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E967" s="5" t="s">
         <v>1276</v>
@@ -30522,7 +30516,7 @@
         <v>1167</v>
       </c>
       <c r="D968" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E968" s="5" t="s">
         <v>1276</v>
@@ -30555,7 +30549,7 @@
         <v>1167</v>
       </c>
       <c r="D969" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E969" s="5" t="s">
         <v>1276</v>
@@ -30588,7 +30582,7 @@
         <v>1167</v>
       </c>
       <c r="D970" s="7" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E970" s="5" t="s">
         <v>1276</v>
@@ -33126,7 +33120,7 @@
         <v>1167</v>
       </c>
       <c r="D1072" s="7" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="E1072" s="5" t="s">
         <v>1250</v>
@@ -33145,7 +33139,7 @@
       <c r="K1072" s="5"/>
       <c r="L1072" s="5"/>
       <c r="M1072" s="5" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="1073" spans="1:13" x14ac:dyDescent="0.25">
@@ -35111,16 +35105,16 @@
         <v>1167</v>
       </c>
       <c r="D1151" s="7" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="E1151" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1151" s="5" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="G1151" s="5" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="H1151" s="5" t="s">
         <v>1182</v>
@@ -35130,7 +35124,7 @@
       <c r="K1151" s="5"/>
       <c r="L1151" s="5"/>
       <c r="M1151" s="5" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="1152" spans="1:13" x14ac:dyDescent="0.25">
@@ -38361,7 +38355,7 @@
         <v>1167</v>
       </c>
       <c r="D1297" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1297" s="5" t="s">
         <v>1228</v>
@@ -38394,7 +38388,7 @@
         <v>1167</v>
       </c>
       <c r="D1298" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1298" s="5" t="s">
         <v>1228</v>
@@ -38425,7 +38419,7 @@
         <v>1167</v>
       </c>
       <c r="D1299" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1299" s="5" t="s">
         <v>1228</v>
@@ -38456,7 +38450,7 @@
         <v>1167</v>
       </c>
       <c r="D1300" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1300" s="5" t="s">
         <v>1228</v>
@@ -38487,7 +38481,7 @@
         <v>1167</v>
       </c>
       <c r="D1301" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1301" s="5" t="s">
         <v>1228</v>
@@ -38518,7 +38512,7 @@
         <v>1167</v>
       </c>
       <c r="D1302" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1302" s="5" t="s">
         <v>1228</v>
@@ -38549,7 +38543,7 @@
         <v>1167</v>
       </c>
       <c r="D1303" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1303" s="5" t="s">
         <v>1228</v>
@@ -38580,7 +38574,7 @@
         <v>1167</v>
       </c>
       <c r="D1304" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1304" s="5" t="s">
         <v>1228</v>
@@ -38611,18 +38605,20 @@
         <v>1167</v>
       </c>
       <c r="D1305" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1305" s="5" t="s">
         <v>1228</v>
       </c>
       <c r="F1305" s="5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G1305" s="5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="H1305" s="5" t="s">
         <v>1606</v>
       </c>
-      <c r="G1305" s="5" t="s">
-        <v>1607</v>
-      </c>
-      <c r="H1305" s="5"/>
       <c r="I1305" s="5"/>
       <c r="J1305" s="5"/>
       <c r="K1305" s="5"/>
@@ -38642,19 +38638,17 @@
         <v>1167</v>
       </c>
       <c r="D1306" s="7" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E1306" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1306" s="5" t="s">
-        <v>1608</v>
-      </c>
-      <c r="G1306" s="5" t="s">
         <v>1182</v>
       </c>
+      <c r="G1306" s="5"/>
       <c r="H1306" s="5" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="I1306" s="5"/>
       <c r="J1306" s="5"/>
@@ -38864,7 +38858,7 @@
         <v>1167</v>
       </c>
       <c r="D1316" s="7" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="E1316" s="5" t="s">
         <v>1196</v>
@@ -38911,7 +38905,7 @@
         <v>1560</v>
       </c>
       <c r="H1317" s="5" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="I1317" s="5"/>
       <c r="J1317" s="5"/>
@@ -39331,7 +39325,7 @@
         <v>1167</v>
       </c>
       <c r="D1337" s="7" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="E1337" s="5" t="s">
         <v>1196</v>
@@ -39366,7 +39360,7 @@
         <v>1167</v>
       </c>
       <c r="D1338" s="7" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="E1338" s="5" t="s">
         <v>1196</v>
@@ -39378,7 +39372,7 @@
         <v>1560</v>
       </c>
       <c r="H1338" s="5" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="I1338" s="5"/>
       <c r="J1338" s="5"/>
@@ -39399,7 +39393,7 @@
         <v>1167</v>
       </c>
       <c r="D1339" s="5" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="E1339" s="5" t="s">
         <v>1250</v>
@@ -39558,7 +39552,7 @@
       <c r="K1345" s="5"/>
       <c r="L1345" s="5"/>
       <c r="M1345" s="5" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="1346" spans="1:13" x14ac:dyDescent="0.25">
@@ -39635,7 +39629,7 @@
         <v>1167</v>
       </c>
       <c r="D1349" s="7" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="E1349" s="5" t="s">
         <v>1228</v>
@@ -39654,7 +39648,7 @@
       <c r="K1349" s="5"/>
       <c r="L1349" s="5"/>
       <c r="M1349" s="5" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="1350" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -39668,19 +39662,19 @@
         <v>1167</v>
       </c>
       <c r="D1350" s="7" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="E1350" s="5" t="s">
         <v>1228</v>
       </c>
       <c r="F1350" s="5" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="G1350" s="5" t="s">
         <v>1182</v>
       </c>
       <c r="H1350" s="5" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="I1350" s="5"/>
       <c r="J1350" s="5"/>
@@ -39722,7 +39716,7 @@
         <v>1167</v>
       </c>
       <c r="D1352" s="7" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="E1352" s="5" t="s">
         <v>1196</v>
@@ -39741,7 +39735,7 @@
       <c r="K1352" s="5"/>
       <c r="L1352" s="5"/>
       <c r="M1352" s="5" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="1353" spans="1:13" x14ac:dyDescent="0.25">
@@ -39776,7 +39770,7 @@
         <v>1167</v>
       </c>
       <c r="D1354" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1354" s="5" t="s">
         <v>1196</v>
@@ -39809,13 +39803,13 @@
         <v>1167</v>
       </c>
       <c r="D1355" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1355" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1355" s="5" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="G1355" s="5" t="s">
         <v>1182</v>
@@ -39844,13 +39838,13 @@
         <v>1167</v>
       </c>
       <c r="D1356" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1356" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1356" s="5" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="G1356" s="5" t="s">
         <v>1182</v>
@@ -39879,13 +39873,13 @@
         <v>1167</v>
       </c>
       <c r="D1357" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1357" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1357" s="5" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="G1357" s="5" t="s">
         <v>1182</v>
@@ -39914,13 +39908,13 @@
         <v>1167</v>
       </c>
       <c r="D1358" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1358" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1358" s="5" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="G1358" s="5" t="s">
         <v>1182</v>
@@ -39949,13 +39943,13 @@
         <v>1167</v>
       </c>
       <c r="D1359" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1359" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1359" s="5" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="G1359" s="5" t="s">
         <v>1182</v>
@@ -39984,13 +39978,13 @@
         <v>1167</v>
       </c>
       <c r="D1360" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1360" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1360" s="5" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="G1360" s="5" t="s">
         <v>1182</v>
@@ -40019,13 +40013,13 @@
         <v>1167</v>
       </c>
       <c r="D1361" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1361" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1361" s="5" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="G1361" s="5" t="s">
         <v>1182</v>
@@ -40054,13 +40048,13 @@
         <v>1167</v>
       </c>
       <c r="D1362" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1362" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1362" s="5" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="G1362" s="5" t="s">
         <v>1182</v>
@@ -40089,13 +40083,13 @@
         <v>1167</v>
       </c>
       <c r="D1363" s="7" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E1363" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="F1363" s="5" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="G1363" s="5" t="s">
         <v>1182</v>
@@ -40166,7 +40160,7 @@
         <v>1167</v>
       </c>
       <c r="D1366" s="7" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="E1366" s="5" t="s">
         <v>1228</v>
@@ -40199,7 +40193,7 @@
         <v>1167</v>
       </c>
       <c r="D1367" s="7" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="E1367" s="5" t="s">
         <v>1228</v>
@@ -40253,7 +40247,7 @@
         <v>1167</v>
       </c>
       <c r="D1369" s="7" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="E1369" s="5" t="s">
         <v>1228</v>
@@ -40286,19 +40280,19 @@
         <v>1167</v>
       </c>
       <c r="D1370" s="7" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="E1370" s="5" t="s">
         <v>1228</v>
       </c>
       <c r="F1370" s="5" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="G1370" s="5" t="s">
         <v>1182</v>
       </c>
       <c r="H1370" s="5" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="I1370" s="5"/>
       <c r="J1370" s="5"/>
@@ -40361,7 +40355,7 @@
         <v>1167</v>
       </c>
       <c r="D1373" s="7" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="E1373" s="5" t="s">
         <v>1228</v>
@@ -40394,7 +40388,7 @@
         <v>1167</v>
       </c>
       <c r="D1374" s="7" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="E1374" s="5" t="s">
         <v>1228</v>
@@ -40406,7 +40400,7 @@
         <v>1182</v>
       </c>
       <c r="H1374" s="5" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="I1374" s="5"/>
       <c r="J1374" s="5"/>
@@ -40427,13 +40421,13 @@
         <v>1167</v>
       </c>
       <c r="D1375" s="7" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="E1375" s="5" t="s">
         <v>1228</v>
       </c>
       <c r="F1375" s="5" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="G1375" s="5" t="s">
         <v>1182</v>
@@ -40523,7 +40517,7 @@
         <v>1167</v>
       </c>
       <c r="D1379" s="7" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="E1379" s="5" t="s">
         <v>1325</v>
@@ -40535,7 +40529,7 @@
         <v>1182</v>
       </c>
       <c r="H1379" s="5" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="I1379" s="5"/>
       <c r="J1379" s="5"/>
@@ -40556,7 +40550,7 @@
         <v>1167</v>
       </c>
       <c r="D1380" s="7" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="E1380" s="5" t="s">
         <v>1196</v>
@@ -40568,7 +40562,7 @@
         <v>1182</v>
       </c>
       <c r="H1380" s="5" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="I1380" s="5"/>
       <c r="J1380" s="5"/>

</xml_diff>